<commit_message>
css rakenne uusittu kuulumiset ja saalistilastot html-sivut
</commit_message>
<xml_diff>
--- a/template_test/Ohjeita/kuulumiset.xlsx
+++ b/template_test/Ohjeita/kuulumiset.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01 naamisuvanto\naamisuvanto\template_test\Ohjeita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87DA925E-66BC-4080-B914-C23C93111111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FDFF05-B741-4314-BDD1-0F69D62E9034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A9D5E6F-737F-4EF9-B07D-0E2B905FE653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,9 +35,77 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Teaser</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Heading2</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Image text</t>
+  </si>
+  <si>
+    <t>Video text</t>
+  </si>
+  <si>
+    <t>Extra video 1</t>
+  </si>
+  <si>
+    <t>Extra video text 1</t>
+  </si>
+  <si>
+    <t>Heading3</t>
+  </si>
+  <si>
+    <t>Extra video 2</t>
+  </si>
+  <si>
+    <t>Extra video text 2</t>
+  </si>
+  <si>
+    <t>Extra video 3</t>
+  </si>
+  <si>
+    <t>Extra video text 3</t>
+  </si>
+  <si>
+    <t>Extra video 4</t>
+  </si>
+  <si>
+    <t>Extra video text 4</t>
+  </si>
+  <si>
+    <t>file:///C:/01%20naamisuvanto/naamisuvanto/template_test/images/kuulumiset/nokipannukahvit.jpg</t>
+  </si>
+  <si>
+    <t>Nokkipannu kahvit</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>Luonnonlohikannat kasvussa</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +113,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -60,13 +153,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,12 +477,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC915696-027D-4CBB-8F2A-242AA6F3CEE3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>37233</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>37221</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:R1" xr:uid="{F2E1D0D6-28D3-4BB5-B070-8446D405AC65}"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{749F2FD4-DE28-4034-8AFB-6F76886CA6F6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>